<commit_message>
Automating with Windows scheduler
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KENNY\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KENNY\source\repos\VickyAmazonWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34035" windowHeight="13515"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="configuration" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>merchandise</t>
   </si>
@@ -27,10 +27,383 @@
     <t>url</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Dual-Texture-Exfoliating-Scrubber-Exfoliator-Scrubbers/product-reviews/B08ZHKS216/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <t>BPHC056-004</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPHC056-005</t>
+  </si>
+  <si>
+    <t>BPHC056-014</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPPC176-004</t>
+  </si>
+  <si>
+    <t>BPPC176-001</t>
+  </si>
+  <si>
+    <t>BABC042-001</t>
+  </si>
+  <si>
+    <t>BPPC024-P008</t>
+  </si>
+  <si>
+    <t>BPPC024-005</t>
+  </si>
+  <si>
+    <t>BPPC024-011-S</t>
+  </si>
+  <si>
+    <t>BPPC176-006</t>
+  </si>
+  <si>
+    <t>BPHC071-001</t>
+  </si>
+  <si>
+    <t>BPPC024-042</t>
+  </si>
+  <si>
+    <t>HKKDA26-P03</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/myHomeBody-Anti-Frizz-Rapid-Dry-Hair-Drying-Absorbent/product-reviews/B07WF7TVRZ/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/myHomeBody-Anti-Frizz-Rapid-Dry-Hair-Drying-Absorbent/product-reviews/B085ZNLL2H/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Microfiber-Gentle-Drying-Products-Scrunchie/product-reviews/B099ZHNKBG/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Bowknot-Reusable-Stripes-Plastic-Accessories/product-reviews/B099WX937K/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Reusable-Plastic-Shower-Colors-Covers/product-reviews/B099WY1HJQ/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Exfoliating-Squares-Scrubber-Leftover-Exfoliator/product-reviews/B0872W1HC4/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/myHomeBody-Exfoliating-Pocket-Scrubber-BPA-Free/product-reviews/B07WF7NSF5/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Bathing-Natural-Sponges-Infants-Plant-Based/product-reviews/B083NJ5YC5/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKKD362-002</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Hand-Towels-Kitchen-Absorbent-Bathroom/product-reviews/B0872V2QD4/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPPC176-005</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Dual-Textured-Exfoliating-Alternative-Exfoliation-Construction/product-reviews/B09W28C65G/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPPC024-003</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKBA075-002</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Shower-Loofah-Sponge-Scrubber-Luxury/product-reviews/B081ZYBPL2/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>BPPC024-010</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/myHomeBody-Multi-Directional-Bioplastic-Efficient-Draining/product-reviews/B07WD424JC/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/myHomeBody-Premium-Sponge-Loofah-Shower/product-reviews/B088RCST4H/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Loofah-Sponge-Scrubber-Luxury-Exfoliating/product-reviews/B08Y5LNHZP/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Natural-Konjac-Facial-Activated-Charcoal/product-reviews/B07Q3DFCVR/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/myHomeBody-Dual-Texture-Sponge-Facial-2-00/product-reviews/B08PNPRX4C/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/myHomeBody-Exfoliating-Exfoliator-Exfoliation-Lightweight/product-reviews/B08R8PV2JG/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Rollers-Sizes-Extra-Large-Curlers/product-reviews/B08ZHQD82Y/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Luxury-Exfoliator-Texture-Exfoliation-Cleansing/product-reviews/B08PF9SNH4/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Potholders-Accessories-Blue-Aqua-Blush/product-reviews/B09CDGJ6KJ/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKKD087-P01</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Wicker-Storage-Basket-Serving-Garden/product-reviews/B099X2588L/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKKD438-P01</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HHHS018-P01</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAFE005-P01</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPOS151-009</t>
+  </si>
+  <si>
+    <t>HKKD734-P02</t>
+  </si>
+  <si>
+    <t>HKKD734-P03</t>
+  </si>
+  <si>
+    <t>HKKD734-P04</t>
+  </si>
+  <si>
+    <t>HKSO109-007</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPOS193-P01</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>OPOS193-P02</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Rectangle-Utensil-Organizer-Organization-Accessories/product-reviews/B099WZXS5Z/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Laundry-Delicates-Washing-Machine-Zipper/product-reviews/B099WG94B7/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Silicone-Elephant-Waterproof-Feeding-Adjustable/product-reviews/B09HLZY2MJ/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPPC024-007</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Natural-Konjac-Facial-Sponges-Exfoliation/product-reviews/B083NHLDZ6/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKKD596-P01</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Organizer-Kitchen-Organization-Spinning-Non-Skid/product-reviews/B099WY9N9Q/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPPC176-P09</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Exfoliating-Washcloth-Scrubber-Remover-Obsidian/product-reviews/B09CYBHYC8/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKBA075-P03</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Waterfall-Draining-Bathroom-Accessories-Silicone/product-reviews/B09C8GQSJQ/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PSDS083-001</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/myHomeBody-Konjac-Natural-Cleaning-Biodegradable/product-reviews/B089N7QNYG/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKBA022-001</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t>‎</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>OPOS151-001</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Catcher-Strainer-Bathroom-Accessories-Kitchen/product-reviews/B09CGCG3BD/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Organizer-Multi-Compartment-Organizers-Accessories-Organization/product-reviews/B09PL9HWKM/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Organizer-Compartment-Organizers-Accessories-Organization/product-reviews/B09PL9MXGJ/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKKD734-P01</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Round-Placemats-Braided-Attractive-Kitchen/product-reviews/B09L83G7BM/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Round-Placemats-Braided-Attractive-Kitchen/product-reviews/B09L83DB5K/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Leather-Resistant-Placemats-Washable-Wipeable/product-reviews/B09CYN14FT/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Silicone-Resistant-Placemats-Placemat-Eggshell/product-reviews/B09CY4S343/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKKD734-P05</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Vinyl-Resistant-Placemats-Dining-Kitchen/product-reviews/B09CYG5G84/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/myHomeBody-Organizing-Bathroom-Organizers-Decorative/product-reviews/B09CP8GSTZ/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Organizer-Organization-Magazine-Baskets-Storage/product-reviews/B09CYSSJHN/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/myHomeBody-Wicker-Paper-Organizer-Tan/product-reviews/B09CPGBQ7W/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/myHomeBody-Storage-Organizing-Organizer-Organization/product-reviews/B09CPCQQ9J/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPPC266-P06</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPPC266-006</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BPPC266-013</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Bowknot-Reusable-Pattern-Plastic-Accessories/product-reviews/B099WX4NW8/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>BAFE005-P04</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Silicone-Waterproof-Feeding-Adjustable-Babies/product-reviews/B09HM4VGY4/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKKD734-P06</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Resistant-Placemats-Dining-Kitchen-Stripes/product-reviews/B09CYBFZ82/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKKD734-P07</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Resistant-Placemats-Dining-Kitchen-Golden/product-reviews/B09CYKS91S/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Resistant-Placemats-Dining-Kitchen-Stripes/product-reviews/B09CYKZF46/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKKD734-P08</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKSO109-P01</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.amazon.com/myHomeBody-Compartments-Organizing-Organizers-Organization/product-reviews/B09CKZZR5Q/ref=cm_cr_dp_d_show_all_btm?ie=UTF8&amp;reviewerType=all_reviews</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKSO109-P02</t>
   </si>
 </sst>
 </file>
@@ -40,7 +413,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -77,6 +450,36 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="MS Gothic"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -129,8 +532,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -138,16 +541,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -158,6 +555,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -476,30 +880,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E8" sqref="E8"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD3"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="50.5" customWidth="1"/>
-    <col min="2" max="2" width="151.25" style="7" customWidth="1"/>
-    <col min="4" max="4" width="59.125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="14.375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="14.125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="11.875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="12.75" style="7" customWidth="1"/>
+    <col min="2" max="2" width="151.25" style="5" customWidth="1"/>
+    <col min="4" max="4" width="59.125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="14.125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="12.75" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1"/>
@@ -509,20 +913,435 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" ht="31.5" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
+      <c r="B3" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="B10" r:id="rId7"/>
+    <hyperlink ref="B11" r:id="rId8"/>
+    <hyperlink ref="B12" r:id="rId9"/>
+    <hyperlink ref="B13" r:id="rId10"/>
+    <hyperlink ref="B14" r:id="rId11"/>
+    <hyperlink ref="B15" r:id="rId12"/>
+    <hyperlink ref="B16" r:id="rId13"/>
+    <hyperlink ref="B17" r:id="rId14"/>
+    <hyperlink ref="B18" r:id="rId15"/>
+    <hyperlink ref="B19" r:id="rId16"/>
+    <hyperlink ref="B20" r:id="rId17"/>
+    <hyperlink ref="B21" r:id="rId18"/>
+    <hyperlink ref="B22" r:id="rId19"/>
+    <hyperlink ref="B23" r:id="rId20"/>
+    <hyperlink ref="B24" r:id="rId21"/>
+    <hyperlink ref="B25" r:id="rId22"/>
+    <hyperlink ref="B26" r:id="rId23"/>
+    <hyperlink ref="B27" r:id="rId24"/>
+    <hyperlink ref="B28" r:id="rId25"/>
+    <hyperlink ref="B29" r:id="rId26"/>
+    <hyperlink ref="B30" r:id="rId27"/>
+    <hyperlink ref="B31" r:id="rId28"/>
+    <hyperlink ref="B32" r:id="rId29"/>
+    <hyperlink ref="B33" r:id="rId30"/>
+    <hyperlink ref="B34" r:id="rId31"/>
+    <hyperlink ref="B35" r:id="rId32"/>
+    <hyperlink ref="B36" r:id="rId33"/>
+    <hyperlink ref="B37" r:id="rId34"/>
+    <hyperlink ref="B38" r:id="rId35"/>
+    <hyperlink ref="B39" r:id="rId36"/>
+    <hyperlink ref="B40" r:id="rId37"/>
+    <hyperlink ref="B45" r:id="rId38"/>
+    <hyperlink ref="B47" r:id="rId39"/>
+    <hyperlink ref="B48" r:id="rId40"/>
+    <hyperlink ref="B44" r:id="rId41"/>
+    <hyperlink ref="B6" r:id="rId42"/>
+    <hyperlink ref="B7" r:id="rId43"/>
+    <hyperlink ref="B41" r:id="rId44"/>
+    <hyperlink ref="B42" r:id="rId45"/>
+    <hyperlink ref="B43" r:id="rId46"/>
+    <hyperlink ref="B46" r:id="rId47"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId48"/>
 </worksheet>
 </file>
</xml_diff>